<commit_message>
Add more info to cheat sheets
</commit_message>
<xml_diff>
--- a/cli_cheat_sheet.xlsx
+++ b/cli_cheat_sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/Desktop/Websites/TUTORIALS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/Websites/TUTORIALS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71ACB3D9-49B2-0041-8922-33BEE6FC32FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75201662-1291-AE4A-BCBF-C92297CF8720}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" xr2:uid="{FC15A83D-849E-144A-99E6-DA158C2BF8E4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="190">
   <si>
     <t>Command</t>
   </si>
@@ -564,6 +564,126 @@
       </rPr>
       <t>cmd2</t>
     </r>
+  </si>
+  <si>
+    <t>mkdir &lt;name&gt;</t>
+  </si>
+  <si>
+    <t>Make directory with name</t>
+  </si>
+  <si>
+    <t>$ mkdir foo</t>
+  </si>
+  <si>
+    <t>pwd</t>
+  </si>
+  <si>
+    <t>Print working directory</t>
+  </si>
+  <si>
+    <t>$ pwd</t>
+  </si>
+  <si>
+    <t>cd &lt;dir&gt;</t>
+  </si>
+  <si>
+    <t>Change to &lt;dir&gt;</t>
+  </si>
+  <si>
+    <t>$ cd foo/</t>
+  </si>
+  <si>
+    <t>cd ~/&lt;dir&gt;</t>
+  </si>
+  <si>
+    <t>cd relative to home</t>
+  </si>
+  <si>
+    <t>$ cd ~/foo/</t>
+  </si>
+  <si>
+    <t>cd</t>
+  </si>
+  <si>
+    <t>Change to home directory</t>
+  </si>
+  <si>
+    <t>$ cd</t>
+  </si>
+  <si>
+    <t>cd -</t>
+  </si>
+  <si>
+    <t>Change to previous directory</t>
+  </si>
+  <si>
+    <t>$ cd &amp;&amp; pwd &amp;&amp; cd -</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>The current directory</t>
+  </si>
+  <si>
+    <t>$ cp ~/foo.txt .</t>
+  </si>
+  <si>
+    <t>..</t>
+  </si>
+  <si>
+    <t>One directory up</t>
+  </si>
+  <si>
+    <t>$ cd ..</t>
+  </si>
+  <si>
+    <t>find</t>
+  </si>
+  <si>
+    <t>Find files &amp; directories</t>
+  </si>
+  <si>
+    <t>$ find . -name foo*.*</t>
+  </si>
+  <si>
+    <t>cp -r &lt;old&gt; &lt;new&gt;</t>
+  </si>
+  <si>
+    <t>Copy recursively</t>
+  </si>
+  <si>
+    <t>$ cp -r ~/foo .</t>
+  </si>
+  <si>
+    <t>rmdir &lt;dir&gt;</t>
+  </si>
+  <si>
+    <t>Remove (empty) dir</t>
+  </si>
+  <si>
+    <t>$ rmdir foo/</t>
+  </si>
+  <si>
+    <t>rm -rf &lt;dir&gt;</t>
+  </si>
+  <si>
+    <t>Remove dir &amp; contents</t>
+  </si>
+  <si>
+    <t>$ rm -rf foo/</t>
+  </si>
+  <si>
+    <t>grep -ri &lt;string&gt; &lt;dir&gt;</t>
+  </si>
+  <si>
+    <t>Grep recursively (case-insensitive)</t>
+  </si>
+  <si>
+    <t>$ grep -ri foo bar/</t>
+  </si>
+  <si>
+    <t>4. Directories</t>
   </si>
 </sst>
 </file>
@@ -688,27 +808,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1023,10 +1146,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18C3F754-B3FA-7B46-9727-781B31049190}">
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1038,88 +1161,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="7"/>
+      <c r="B1" s="13"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>45</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>46</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>48</v>
       </c>
       <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>50</v>
       </c>
       <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>54</v>
       </c>
       <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>56</v>
       </c>
       <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>58</v>
       </c>
       <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="7" t="s">
         <v>60</v>
       </c>
       <c r="C10" s="4"/>
@@ -1130,120 +1253,120 @@
       <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="7"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="9" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="9" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="9" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="9"/>
+      <c r="C17" s="7"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="9"/>
+      <c r="C18" s="7"/>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="9"/>
+      <c r="C19" s="7"/>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C20" s="9"/>
+      <c r="C20" s="7"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C21" s="9"/>
+      <c r="C21" s="7"/>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="9" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="9" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1253,163 +1376,163 @@
       <c r="C24" s="4"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="7"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="13"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="9" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="9" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="9" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="9" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="9" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="9" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="11" t="s">
+      <c r="A34" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="9" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="9" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="11" t="s">
+      <c r="A36" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C36" s="9" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="11" t="s">
+      <c r="A37" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C37" s="9" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="11" t="s">
+      <c r="A38" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C38" s="9" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="11" t="s">
+      <c r="A39" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C39" s="9" t="s">
         <v>122</v>
       </c>
     </row>
@@ -1419,275 +1542,437 @@
       <c r="C40" s="4"/>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="B41" s="10"/>
-      <c r="C41" s="7"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="13"/>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="8" t="s">
+      <c r="A42" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B42" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C42" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="B43" s="9" t="s">
+      <c r="B43" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="C43" s="9"/>
+      <c r="C43" s="7"/>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="11" t="s">
+      <c r="A44" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="B44" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="C44" s="9"/>
+      <c r="C44" s="7"/>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="11" t="s">
+      <c r="A45" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B45" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="C45" s="9"/>
+      <c r="C45" s="7"/>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="11" t="s">
+      <c r="A46" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="C46" s="9"/>
+      <c r="C46" s="7"/>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="11" t="s">
+      <c r="A47" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="B47" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="C47" s="9"/>
+      <c r="C47" s="7"/>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="11" t="s">
+      <c r="A48" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="C48" s="9"/>
+      <c r="C48" s="7"/>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="11" t="s">
+      <c r="A49" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B49" s="9" t="s">
+      <c r="B49" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="C49" s="12" t="s">
+      <c r="C49" s="9" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="11" t="s">
+      <c r="A50" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="B50" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="C50" s="13"/>
+      <c r="C50" s="10"/>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="11" t="s">
+      <c r="A51" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="B51" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="C51" s="13"/>
+      <c r="C51" s="10"/>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="11" t="s">
+      <c r="A52" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="B52" s="9" t="s">
+      <c r="B52" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="C52" s="13"/>
+      <c r="C52" s="10"/>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="11" t="s">
+      <c r="A53" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B53" s="9" t="s">
+      <c r="B53" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C53" s="12" t="s">
+      <c r="C53" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="11" t="s">
+      <c r="A54" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B54" s="9" t="s">
+      <c r="B54" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C54" s="12" t="s">
+      <c r="C54" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="11" t="s">
+      <c r="A55" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B55" s="9" t="s">
+      <c r="B55" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C55" s="12" t="s">
+      <c r="C55" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" s="11" t="s">
+      <c r="A56" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B56" s="9" t="s">
+      <c r="B56" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C56" s="12" t="s">
+      <c r="C56" s="9" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" s="11" t="s">
+      <c r="A57" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B57" s="9" t="s">
+      <c r="B57" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C57" s="12" t="s">
+      <c r="C57" s="9" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" s="11" t="s">
+      <c r="A58" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B58" s="9" t="s">
+      <c r="B58" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="C58" s="12" t="s">
+      <c r="C58" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" s="11" t="s">
+      <c r="A59" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B59" s="9" t="s">
+      <c r="B59" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C59" s="12" t="s">
+      <c r="C59" s="9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="11" t="s">
+      <c r="A60" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B60" s="9" t="s">
+      <c r="B60" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C60" s="12" t="s">
+      <c r="C60" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="11" t="s">
+      <c r="A61" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B61" s="9" t="s">
+      <c r="B61" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C61" s="12" t="s">
+      <c r="C61" s="9" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="11" t="s">
+      <c r="A62" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B62" s="9" t="s">
+      <c r="B62" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C62" s="12" t="s">
+      <c r="C62" s="9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" s="11" t="s">
+      <c r="A63" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B63" s="9" t="s">
+      <c r="B63" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C63" s="12" t="s">
+      <c r="C63" s="9" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" s="11" t="s">
+      <c r="A64" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B64" s="9" t="s">
+      <c r="B64" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C64" s="12" t="s">
+      <c r="C64" s="9" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" s="11" t="s">
+      <c r="A65" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B65" s="9" t="s">
+      <c r="B65" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C65" s="12" t="s">
+      <c r="C65" s="9" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="11" t="s">
+      <c r="A66" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B66" s="9" t="s">
+      <c r="B66" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C66" s="12" t="s">
+      <c r="C66" s="9" t="s">
         <v>43</v>
       </c>
     </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="B68" s="14"/>
+      <c r="C68" s="14"/>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C77" s="9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C79" s="9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C80" s="9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C81" s="9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C82" s="9" t="s">
+        <v>188</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A41:C41"/>
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A68:C68"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>